<commit_message>
Add HTML templates for Visage and update attendance data format
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,155 +453,106 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CHARLES LECLERC</t>
+          <t>DENZEL WASHINGTON</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2023-10-01</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>20:21:16</t>
-        </is>
-      </c>
+          <t xml:space="preserve"> 01:44:04</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>JEFF BESOS</t>
+          <t>CHARLES LECLERC</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2023-10-01</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>20:21:39</t>
-        </is>
-      </c>
+          <t xml:space="preserve"> 01:44:59</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>JENSEN HUANG</t>
+          <t>TOM CRUISE</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2023-10-01</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>20:21:59</t>
-        </is>
-      </c>
+          <t xml:space="preserve"> 02:15:22</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>STEVE JOBS</t>
+          <t>JEFF BESOS</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2023-10-01</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>20:23:13</t>
-        </is>
-      </c>
+          <t xml:space="preserve"> 02:16:02</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DENZEL WASHINGTON</t>
+          <t>LEO MESSI</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2023-10-01</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>20:23:34</t>
-        </is>
-      </c>
+          <t xml:space="preserve"> 02:16:19</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SAM ALTMAN</t>
+          <t>NELSON MANDELA</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2023-10-01</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>20:24:01</t>
-        </is>
-      </c>
+          <t xml:space="preserve"> 02:16:35</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LEO MESSI</t>
+          <t>SAM ALTMAN</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2023-10-01</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>20:25:35</t>
-        </is>
-      </c>
+          <t xml:space="preserve"> 02:17:05</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>TOM CRUISE</t>
+          <t>STEVE JOBS</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2023-10-01</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>20:26:20</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>NELSON MANDELA</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2023-10-01</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>20:26:56</t>
-        </is>
-      </c>
+          <t xml:space="preserve"> 02:27:45</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>